<commit_message>
add script to turn table into plate
</commit_message>
<xml_diff>
--- a/PeptideRegisCode/Order.xlsx
+++ b/PeptideRegisCode/Order.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E4D668-D7D8-4BB1-A989-E20FE4875D05}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928C0D09-F9DF-4F9A-93BA-0CF37731357D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5366" uniqueCount="3233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5368" uniqueCount="3235">
   <si>
     <t xml:space="preserve">1	</t>
   </si>
@@ -9714,6 +9714,12 @@
   </si>
   <si>
     <t>1.0mg</t>
+  </si>
+  <si>
+    <t>Source Protein</t>
+  </si>
+  <si>
+    <t>UniProt ID</t>
   </si>
 </sst>
 </file>
@@ -10096,18 +10102,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1073"/>
+  <dimension ref="A1:H1073"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I330" sqref="I330"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>2144</v>
       </c>
@@ -10126,8 +10138,14 @@
       <c r="F1" t="s">
         <v>2149</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>3233</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>2150</v>
       </c>
@@ -10147,7 +10165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2151</v>
       </c>
@@ -10167,7 +10185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>2152</v>
       </c>
@@ -10187,7 +10205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>2153</v>
       </c>
@@ -10207,7 +10225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>2154</v>
       </c>
@@ -10227,7 +10245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>2155</v>
       </c>
@@ -10247,7 +10265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>2156</v>
       </c>
@@ -10267,7 +10285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>2157</v>
       </c>
@@ -10287,7 +10305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>2158</v>
       </c>
@@ -10307,7 +10325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>2159</v>
       </c>
@@ -10327,7 +10345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>2160</v>
       </c>
@@ -10347,7 +10365,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>2161</v>
       </c>
@@ -10367,7 +10385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>2162</v>
       </c>
@@ -10387,7 +10405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>2163</v>
       </c>
@@ -10407,7 +10425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>2164</v>
       </c>

</xml_diff>